<commit_message>
updates to the 2024 data
</commit_message>
<xml_diff>
--- a/sccj-faculty-salary-data.xlsx
+++ b/sccj-faculty-salary-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyoung20/GitHub/sccj-faculty-salary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jyoung20/Github/sccj-faculty-salary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964B339D-1331-0549-ABE4-0D8263044727}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBFE5F26-C1EE-D546-912C-EFF82B253D9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18240" xr2:uid="{390A8155-8037-4544-B779-6A79251AF3D7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="40960" windowHeight="21720" xr2:uid="{390A8155-8037-4544-B779-6A79251AF3D7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1001" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1161" uniqueCount="112">
   <si>
     <t>ID</t>
   </si>
@@ -362,6 +362,15 @@
   </si>
   <si>
     <t>Peguero</t>
+  </si>
+  <si>
+    <t>JW</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>WrightJ</t>
   </si>
 </sst>
 </file>
@@ -721,10 +730,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{718F963D-5933-5B4F-9721-1D63B7B62310}">
-  <dimension ref="A1:H192"/>
+  <dimension ref="A1:H224"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" zoomScale="192" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -760,42 +769,42 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="B2">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>110</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>111</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F2">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
       </c>
       <c r="H2">
-        <v>90000</v>
+        <v>145000</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -804,24 +813,24 @@
         <v>2022</v>
       </c>
       <c r="G3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H3">
-        <v>92000</v>
+        <v>94500</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -833,21 +842,21 @@
         <v>14</v>
       </c>
       <c r="H4">
-        <v>90000</v>
+        <v>92000</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -856,27 +865,27 @@
         <v>2022</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H5">
-        <v>90000</v>
+        <v>94500</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F6">
         <v>2022</v>
@@ -885,21 +894,21 @@
         <v>11</v>
       </c>
       <c r="H6">
-        <v>120000</v>
+        <v>95500</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C7" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E7" t="s">
         <v>21</v>
@@ -908,414 +917,414 @@
         <v>2022</v>
       </c>
       <c r="G7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H7">
-        <v>200000</v>
+        <v>122500</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F8">
-        <v>2012</v>
+        <v>2022</v>
       </c>
       <c r="G8" t="s">
         <v>14</v>
       </c>
       <c r="H8">
-        <v>110000</v>
+        <v>204000</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F9">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H9">
-        <v>102000</v>
+        <v>114000</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E10" t="s">
         <v>21</v>
       </c>
       <c r="F10">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="G10" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H10">
-        <v>120016</v>
+        <v>133056</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
       <c r="F11">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H11">
-        <v>151000</v>
+        <v>125016</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B12">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E12" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H12">
-        <v>92000</v>
+        <v>154200</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B13">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E13" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F13">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="G13" t="s">
         <v>14</v>
       </c>
       <c r="H13">
-        <v>127000</v>
+        <v>96500</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B14">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
         <v>21</v>
       </c>
       <c r="F14">
-        <v>1997</v>
+        <v>2008</v>
       </c>
       <c r="G14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H14">
-        <v>180800</v>
+        <v>130200</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B15">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
       </c>
       <c r="F15">
-        <v>2016</v>
+        <v>1997</v>
       </c>
       <c r="G15" t="s">
         <v>11</v>
       </c>
       <c r="H15">
-        <v>169300</v>
+        <v>184000</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B16">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D16" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F16">
-        <v>2018</v>
+        <v>2016</v>
       </c>
       <c r="G16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H16">
-        <v>95000</v>
+        <v>172500</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="F17">
-        <v>2015</v>
+        <v>2018</v>
       </c>
       <c r="G17" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H17">
-        <v>146144</v>
+        <v>106300</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
         <v>21</v>
       </c>
       <c r="F18">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" t="s">
-        <v>73</v>
+      <c r="H18">
+        <v>149700</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
       <c r="F19">
-        <v>2015</v>
+        <v>2020</v>
       </c>
       <c r="G19" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H19">
-        <v>120000</v>
+        <v>185600</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B20">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E20" t="s">
         <v>21</v>
       </c>
       <c r="F20">
-        <v>2008</v>
+        <v>2015</v>
       </c>
       <c r="G20" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H20">
-        <v>147646</v>
+        <v>125000</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B21">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F21">
-        <v>2015</v>
+        <v>2008</v>
       </c>
       <c r="G21" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H21">
-        <v>107000</v>
+        <v>150846</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B22">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="F22">
-        <v>2006</v>
+        <v>2015</v>
       </c>
       <c r="G22" t="s">
         <v>14</v>
       </c>
       <c r="H22">
-        <v>230000</v>
+        <v>111000</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
@@ -1324,154 +1333,154 @@
         <v>2006</v>
       </c>
       <c r="G23" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H23">
-        <v>119921</v>
+        <v>231500</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B24">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D24" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F24">
-        <v>2013</v>
+        <v>2006</v>
       </c>
       <c r="G24" t="s">
         <v>11</v>
       </c>
       <c r="H24">
-        <v>110000</v>
+        <v>122921</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B25">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E25" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="F25">
-        <v>2015</v>
+        <v>2013</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
       </c>
       <c r="H25">
-        <v>197500</v>
+        <v>116000</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B26">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E26" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F26">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="G26" t="s">
         <v>11</v>
       </c>
       <c r="H26">
-        <v>103000</v>
+        <v>203500</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B27">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E27" t="s">
         <v>74</v>
       </c>
       <c r="F27">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H27">
-        <v>110060</v>
+        <v>106000</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B28">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E28" t="s">
-        <v>21</v>
+        <v>74</v>
       </c>
       <c r="F28">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="G28" t="s">
         <v>14</v>
       </c>
       <c r="H28">
-        <v>120063</v>
+        <v>114060</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="D29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E29" t="s">
         <v>21</v>
@@ -1480,128 +1489,128 @@
         <v>2008</v>
       </c>
       <c r="G29" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H29">
-        <v>180538</v>
+        <v>123063</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B30">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F30">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="G30" t="s">
         <v>11</v>
       </c>
       <c r="H30">
-        <v>112316</v>
+        <v>183913</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B31">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C31" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E31" t="s">
         <v>74</v>
       </c>
       <c r="F31">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="G31" t="s">
         <v>11</v>
       </c>
       <c r="H31">
-        <v>95000</v>
+        <v>115316</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="C32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E32" t="s">
         <v>74</v>
       </c>
       <c r="F32">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="G32" t="s">
         <v>11</v>
       </c>
       <c r="H32">
-        <v>110017</v>
+        <v>106000</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
       <c r="B33">
-        <v>2022</v>
+        <v>2024</v>
       </c>
       <c r="C33" t="s">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>72</v>
       </c>
       <c r="E33" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F33">
-        <v>2022</v>
+        <v>2011</v>
       </c>
       <c r="G33" t="s">
         <v>11</v>
       </c>
       <c r="H33">
-        <v>90000</v>
+        <v>113017</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C34" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D34" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
         <v>10</v>
@@ -1610,24 +1619,24 @@
         <v>2022</v>
       </c>
       <c r="G34" t="s">
-        <v>14</v>
-      </c>
-      <c r="H34" t="s">
-        <v>73</v>
+        <v>11</v>
+      </c>
+      <c r="H34">
+        <v>90000</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B35">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C35" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D35" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E35" t="s">
         <v>10</v>
@@ -1639,21 +1648,21 @@
         <v>14</v>
       </c>
       <c r="H35">
-        <v>90000</v>
+        <v>92000</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B36">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C36" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D36" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E36" t="s">
         <v>10</v>
@@ -1662,7 +1671,7 @@
         <v>2022</v>
       </c>
       <c r="G36" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H36">
         <v>90000</v>
@@ -1670,19 +1679,19 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B37">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C37" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E37" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F37">
         <v>2022</v>
@@ -1690,22 +1699,22 @@
       <c r="G37" t="s">
         <v>11</v>
       </c>
-      <c r="H37" t="s">
-        <v>73</v>
+      <c r="H37">
+        <v>90000</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B38">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C38" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
+        <v>20</v>
       </c>
       <c r="E38" t="s">
         <v>21</v>
@@ -1714,244 +1723,244 @@
         <v>2022</v>
       </c>
       <c r="G38" t="s">
-        <v>14</v>
-      </c>
-      <c r="H38" t="s">
-        <v>73</v>
+        <v>11</v>
+      </c>
+      <c r="H38">
+        <v>120000</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B39">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C39" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s">
-        <v>24</v>
+        <v>107</v>
       </c>
       <c r="E39" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F39">
-        <v>2012</v>
+        <v>2022</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
       </c>
       <c r="H39">
-        <v>104000</v>
+        <v>200000</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B40">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C40" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D40" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E40" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F40">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="G40" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H40">
-        <v>102000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C41" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D41" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E41" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F41">
-        <v>2012</v>
+        <v>2018</v>
       </c>
       <c r="G41" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H41">
-        <v>114716</v>
+        <v>102000</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C42" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E42" t="s">
         <v>21</v>
       </c>
       <c r="F42">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="G42" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H42">
-        <v>148500</v>
+        <v>120016</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D43" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E43" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="F43">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="G43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="H43">
-        <v>86000</v>
+        <v>151000</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B44">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C44" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E44" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="F44">
-        <v>2008</v>
+        <v>2020</v>
       </c>
       <c r="G44" t="s">
         <v>14</v>
       </c>
       <c r="H44">
-        <v>123000</v>
+        <v>92000</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B45">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C45" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D45" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
         <v>21</v>
       </c>
       <c r="F45">
-        <v>1997</v>
+        <v>2008</v>
       </c>
       <c r="G45" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H45">
-        <v>168300</v>
+        <v>127000</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B46">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C46" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D46" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E46" t="s">
         <v>21</v>
       </c>
       <c r="F46">
-        <v>2016</v>
+        <v>1997</v>
       </c>
       <c r="G46" t="s">
         <v>11</v>
       </c>
       <c r="H46">
-        <v>166800</v>
+        <v>180800</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B47">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E47" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F47">
-        <v>2020</v>
+        <v>2016</v>
       </c>
       <c r="G47" t="s">
         <v>11</v>
       </c>
       <c r="H47">
-        <v>112200</v>
+        <v>169300</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -1959,7 +1968,7 @@
         <v>90</v>
       </c>
       <c r="B48">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C48" t="s">
         <v>41</v>
@@ -1977,7 +1986,7 @@
         <v>14</v>
       </c>
       <c r="H48">
-        <v>90000</v>
+        <v>95000</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
@@ -1985,7 +1994,7 @@
         <v>91</v>
       </c>
       <c r="B49">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C49" t="s">
         <v>43</v>
@@ -2003,7 +2012,7 @@
         <v>11</v>
       </c>
       <c r="H49">
-        <v>143336</v>
+        <v>146144</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2011,7 +2020,7 @@
         <v>92</v>
       </c>
       <c r="B50">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C50" t="s">
         <v>45</v>
@@ -2028,8 +2037,8 @@
       <c r="G50" t="s">
         <v>11</v>
       </c>
-      <c r="H50">
-        <v>152490</v>
+      <c r="H50" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
@@ -2037,7 +2046,7 @@
         <v>93</v>
       </c>
       <c r="B51">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C51" t="s">
         <v>46</v>
@@ -2055,7 +2064,7 @@
         <v>14</v>
       </c>
       <c r="H51">
-        <v>115500</v>
+        <v>120000</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
@@ -2063,7 +2072,7 @@
         <v>94</v>
       </c>
       <c r="B52">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C52" t="s">
         <v>48</v>
@@ -2081,7 +2090,7 @@
         <v>11</v>
       </c>
       <c r="H52">
-        <v>145146</v>
+        <v>147646</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
@@ -2089,7 +2098,7 @@
         <v>95</v>
       </c>
       <c r="B53">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
@@ -2107,7 +2116,7 @@
         <v>14</v>
       </c>
       <c r="H53">
-        <v>100000</v>
+        <v>107000</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
@@ -2115,7 +2124,7 @@
         <v>96</v>
       </c>
       <c r="B54">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C54" t="s">
         <v>52</v>
@@ -2141,7 +2150,7 @@
         <v>97</v>
       </c>
       <c r="B55">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C55" t="s">
         <v>54</v>
@@ -2150,7 +2159,7 @@
         <v>55</v>
       </c>
       <c r="E55" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F55">
         <v>2006</v>
@@ -2159,7 +2168,7 @@
         <v>11</v>
       </c>
       <c r="H55">
-        <v>105019</v>
+        <v>119921</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
@@ -2167,7 +2176,7 @@
         <v>98</v>
       </c>
       <c r="B56">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C56" t="s">
         <v>56</v>
@@ -2185,7 +2194,7 @@
         <v>11</v>
       </c>
       <c r="H56">
-        <v>104000</v>
+        <v>110000</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
@@ -2193,7 +2202,7 @@
         <v>99</v>
       </c>
       <c r="B57">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C57" t="s">
         <v>58</v>
@@ -2211,7 +2220,7 @@
         <v>11</v>
       </c>
       <c r="H57">
-        <v>195000</v>
+        <v>197500</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
@@ -2219,7 +2228,7 @@
         <v>100</v>
       </c>
       <c r="B58">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C58" t="s">
         <v>60</v>
@@ -2228,7 +2237,7 @@
         <v>61</v>
       </c>
       <c r="E58" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F58">
         <v>2016</v>
@@ -2237,7 +2246,7 @@
         <v>11</v>
       </c>
       <c r="H58">
-        <v>87000</v>
+        <v>103000</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
@@ -2245,7 +2254,7 @@
         <v>101</v>
       </c>
       <c r="B59">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C59" t="s">
         <v>62</v>
@@ -2263,7 +2272,7 @@
         <v>14</v>
       </c>
       <c r="H59">
-        <v>105060</v>
+        <v>110060</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
@@ -2271,7 +2280,7 @@
         <v>102</v>
       </c>
       <c r="B60">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C60" t="s">
         <v>64</v>
@@ -2280,7 +2289,7 @@
         <v>65</v>
       </c>
       <c r="E60" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F60">
         <v>2008</v>
@@ -2289,7 +2298,7 @@
         <v>14</v>
       </c>
       <c r="H60">
-        <v>103148</v>
+        <v>120063</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
@@ -2297,7 +2306,7 @@
         <v>103</v>
       </c>
       <c r="B61">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C61" t="s">
         <v>48</v>
@@ -2315,7 +2324,7 @@
         <v>11</v>
       </c>
       <c r="H61">
-        <v>178038</v>
+        <v>180538</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -2323,7 +2332,7 @@
         <v>104</v>
       </c>
       <c r="B62">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C62" t="s">
         <v>67</v>
@@ -2341,7 +2350,7 @@
         <v>11</v>
       </c>
       <c r="H62">
-        <v>109315</v>
+        <v>112316</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
@@ -2349,7 +2358,7 @@
         <v>105</v>
       </c>
       <c r="B63">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C63" t="s">
         <v>69</v>
@@ -2358,7 +2367,7 @@
         <v>70</v>
       </c>
       <c r="E63" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F63">
         <v>2016</v>
@@ -2367,7 +2376,7 @@
         <v>11</v>
       </c>
       <c r="H63">
-        <v>87000</v>
+        <v>95000</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
@@ -2375,7 +2384,7 @@
         <v>106</v>
       </c>
       <c r="B64">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="C64" t="s">
         <v>71</v>
@@ -2393,7 +2402,7 @@
         <v>11</v>
       </c>
       <c r="H64">
-        <v>104017</v>
+        <v>110017</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
@@ -2401,7 +2410,7 @@
         <v>75</v>
       </c>
       <c r="B65">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C65" t="s">
         <v>8</v>
@@ -2418,8 +2427,8 @@
       <c r="G65" t="s">
         <v>11</v>
       </c>
-      <c r="H65" t="s">
-        <v>73</v>
+      <c r="H65">
+        <v>90000</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -2427,7 +2436,7 @@
         <v>76</v>
       </c>
       <c r="B66">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C66" t="s">
         <v>12</v>
@@ -2453,7 +2462,7 @@
         <v>77</v>
       </c>
       <c r="B67">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C67" t="s">
         <v>15</v>
@@ -2470,8 +2479,8 @@
       <c r="G67" t="s">
         <v>14</v>
       </c>
-      <c r="H67" t="s">
-        <v>73</v>
+      <c r="H67">
+        <v>90000</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2479,7 +2488,7 @@
         <v>78</v>
       </c>
       <c r="B68">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C68" t="s">
         <v>17</v>
@@ -2496,8 +2505,8 @@
       <c r="G68" t="s">
         <v>11</v>
       </c>
-      <c r="H68" t="s">
-        <v>73</v>
+      <c r="H68">
+        <v>90000</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
@@ -2505,7 +2514,7 @@
         <v>79</v>
       </c>
       <c r="B69">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C69" t="s">
         <v>19</v>
@@ -2531,7 +2540,7 @@
         <v>80</v>
       </c>
       <c r="B70">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C70" t="s">
         <v>22</v>
@@ -2557,7 +2566,7 @@
         <v>81</v>
       </c>
       <c r="B71">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C71" t="s">
         <v>23</v>
@@ -2583,7 +2592,7 @@
         <v>82</v>
       </c>
       <c r="B72">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C72" t="s">
         <v>25</v>
@@ -2601,7 +2610,7 @@
         <v>11</v>
       </c>
       <c r="H72">
-        <v>94000</v>
+        <v>102000</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2609,7 +2618,7 @@
         <v>83</v>
       </c>
       <c r="B73">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C73" t="s">
         <v>27</v>
@@ -2635,7 +2644,7 @@
         <v>84</v>
       </c>
       <c r="B74">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C74" t="s">
         <v>29</v>
@@ -2661,7 +2670,7 @@
         <v>85</v>
       </c>
       <c r="B75">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C75" t="s">
         <v>31</v>
@@ -2687,7 +2696,7 @@
         <v>86</v>
       </c>
       <c r="B76">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C76" t="s">
         <v>33</v>
@@ -2695,7 +2704,7 @@
       <c r="D76" t="s">
         <v>34</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="E76" t="s">
         <v>21</v>
       </c>
       <c r="F76">
@@ -2713,7 +2722,7 @@
         <v>87</v>
       </c>
       <c r="B77">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C77" t="s">
         <v>35</v>
@@ -2721,7 +2730,7 @@
       <c r="D77" t="s">
         <v>36</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E77" t="s">
         <v>21</v>
       </c>
       <c r="F77">
@@ -2739,7 +2748,7 @@
         <v>88</v>
       </c>
       <c r="B78">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C78" t="s">
         <v>37</v>
@@ -2747,7 +2756,7 @@
       <c r="D78" t="s">
         <v>38</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="E78" t="s">
         <v>21</v>
       </c>
       <c r="F78">
@@ -2757,7 +2766,7 @@
         <v>11</v>
       </c>
       <c r="H78">
-        <v>168800</v>
+        <v>166800</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2765,7 +2774,7 @@
         <v>89</v>
       </c>
       <c r="B79">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C79" t="s">
         <v>39</v>
@@ -2773,7 +2782,7 @@
       <c r="D79" t="s">
         <v>40</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="E79" t="s">
         <v>74</v>
       </c>
       <c r="F79">
@@ -2791,7 +2800,7 @@
         <v>90</v>
       </c>
       <c r="B80">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C80" t="s">
         <v>41</v>
@@ -2799,7 +2808,7 @@
       <c r="D80" t="s">
         <v>42</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="E80" t="s">
         <v>10</v>
       </c>
       <c r="F80">
@@ -2817,7 +2826,7 @@
         <v>91</v>
       </c>
       <c r="B81">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C81" t="s">
         <v>43</v>
@@ -2825,7 +2834,7 @@
       <c r="D81" t="s">
         <v>44</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="E81" t="s">
         <v>21</v>
       </c>
       <c r="F81">
@@ -2835,7 +2844,7 @@
         <v>11</v>
       </c>
       <c r="H81">
-        <v>143367</v>
+        <v>143336</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2843,7 +2852,7 @@
         <v>92</v>
       </c>
       <c r="B82">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C82" t="s">
         <v>45</v>
@@ -2869,7 +2878,7 @@
         <v>93</v>
       </c>
       <c r="B83">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C83" t="s">
         <v>46</v>
@@ -2878,7 +2887,7 @@
         <v>47</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F83">
         <v>2015</v>
@@ -2887,7 +2896,7 @@
         <v>14</v>
       </c>
       <c r="H83">
-        <v>105000</v>
+        <v>115500</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2895,7 +2904,7 @@
         <v>94</v>
       </c>
       <c r="B84">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C84" t="s">
         <v>48</v>
@@ -2903,7 +2912,7 @@
       <c r="D84" t="s">
         <v>49</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="E84" t="s">
         <v>21</v>
       </c>
       <c r="F84">
@@ -2921,7 +2930,7 @@
         <v>95</v>
       </c>
       <c r="B85">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C85" t="s">
         <v>50</v>
@@ -2929,7 +2938,7 @@
       <c r="D85" t="s">
         <v>51</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E85" t="s">
         <v>74</v>
       </c>
       <c r="F85">
@@ -2947,7 +2956,7 @@
         <v>96</v>
       </c>
       <c r="B86">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C86" t="s">
         <v>52</v>
@@ -2955,7 +2964,7 @@
       <c r="D86" t="s">
         <v>53</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="E86" t="s">
         <v>21</v>
       </c>
       <c r="F86">
@@ -2973,7 +2982,7 @@
         <v>97</v>
       </c>
       <c r="B87">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C87" t="s">
         <v>54</v>
@@ -2981,7 +2990,7 @@
       <c r="D87" t="s">
         <v>55</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="E87" t="s">
         <v>74</v>
       </c>
       <c r="F87">
@@ -2999,7 +3008,7 @@
         <v>98</v>
       </c>
       <c r="B88">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C88" t="s">
         <v>56</v>
@@ -3007,7 +3016,7 @@
       <c r="D88" t="s">
         <v>57</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="E88" t="s">
         <v>74</v>
       </c>
       <c r="F88">
@@ -3025,7 +3034,7 @@
         <v>99</v>
       </c>
       <c r="B89">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C89" t="s">
         <v>58</v>
@@ -3033,7 +3042,7 @@
       <c r="D89" t="s">
         <v>59</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="E89" t="s">
         <v>21</v>
       </c>
       <c r="F89">
@@ -3051,7 +3060,7 @@
         <v>100</v>
       </c>
       <c r="B90">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C90" t="s">
         <v>60</v>
@@ -3059,7 +3068,7 @@
       <c r="D90" t="s">
         <v>61</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="E90" t="s">
         <v>10</v>
       </c>
       <c r="F90">
@@ -3077,7 +3086,7 @@
         <v>101</v>
       </c>
       <c r="B91">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C91" t="s">
         <v>62</v>
@@ -3085,7 +3094,7 @@
       <c r="D91" t="s">
         <v>63</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="E91" t="s">
         <v>74</v>
       </c>
       <c r="F91">
@@ -3103,7 +3112,7 @@
         <v>102</v>
       </c>
       <c r="B92">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C92" t="s">
         <v>64</v>
@@ -3111,7 +3120,7 @@
       <c r="D92" t="s">
         <v>65</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" t="s">
         <v>74</v>
       </c>
       <c r="F92">
@@ -3129,7 +3138,7 @@
         <v>103</v>
       </c>
       <c r="B93">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C93" t="s">
         <v>48</v>
@@ -3137,7 +3146,7 @@
       <c r="D93" t="s">
         <v>66</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="E93" t="s">
         <v>21</v>
       </c>
       <c r="F93">
@@ -3155,7 +3164,7 @@
         <v>104</v>
       </c>
       <c r="B94">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C94" t="s">
         <v>67</v>
@@ -3173,7 +3182,7 @@
         <v>11</v>
       </c>
       <c r="H94">
-        <v>109316</v>
+        <v>109315</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -3181,7 +3190,7 @@
         <v>105</v>
       </c>
       <c r="B95">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C95" t="s">
         <v>69</v>
@@ -3207,7 +3216,7 @@
         <v>106</v>
       </c>
       <c r="B96">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C96" t="s">
         <v>71</v>
@@ -3233,7 +3242,7 @@
         <v>75</v>
       </c>
       <c r="B97">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C97" t="s">
         <v>8</v>
@@ -3259,7 +3268,7 @@
         <v>76</v>
       </c>
       <c r="B98">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C98" t="s">
         <v>12</v>
@@ -3285,7 +3294,7 @@
         <v>77</v>
       </c>
       <c r="B99">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C99" t="s">
         <v>15</v>
@@ -3311,7 +3320,7 @@
         <v>78</v>
       </c>
       <c r="B100">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C100" t="s">
         <v>17</v>
@@ -3337,7 +3346,7 @@
         <v>79</v>
       </c>
       <c r="B101">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C101" t="s">
         <v>19</v>
@@ -3363,7 +3372,7 @@
         <v>80</v>
       </c>
       <c r="B102">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C102" t="s">
         <v>22</v>
@@ -3389,7 +3398,7 @@
         <v>81</v>
       </c>
       <c r="B103">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C103" t="s">
         <v>23</v>
@@ -3407,7 +3416,7 @@
         <v>14</v>
       </c>
       <c r="H103">
-        <v>100000</v>
+        <v>104000</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
@@ -3415,7 +3424,7 @@
         <v>82</v>
       </c>
       <c r="B104">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C104" t="s">
         <v>25</v>
@@ -3433,7 +3442,7 @@
         <v>11</v>
       </c>
       <c r="H104">
-        <v>84000</v>
+        <v>94000</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
@@ -3441,7 +3450,7 @@
         <v>83</v>
       </c>
       <c r="B105">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C105" t="s">
         <v>27</v>
@@ -3450,7 +3459,7 @@
         <v>28</v>
       </c>
       <c r="E105" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F105">
         <v>2012</v>
@@ -3459,7 +3468,7 @@
         <v>14</v>
       </c>
       <c r="H105">
-        <v>101250</v>
+        <v>114716</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
@@ -3467,7 +3476,7 @@
         <v>84</v>
       </c>
       <c r="B106">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C106" t="s">
         <v>29</v>
@@ -3475,7 +3484,7 @@
       <c r="D106" t="s">
         <v>30</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="E106" t="s">
         <v>21</v>
       </c>
       <c r="F106">
@@ -3485,7 +3494,7 @@
         <v>11</v>
       </c>
       <c r="H106">
-        <v>144500</v>
+        <v>148500</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
@@ -3493,7 +3502,7 @@
         <v>85</v>
       </c>
       <c r="B107">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C107" t="s">
         <v>31</v>
@@ -3510,8 +3519,8 @@
       <c r="G107" t="s">
         <v>14</v>
       </c>
-      <c r="H107" t="s">
-        <v>73</v>
+      <c r="H107">
+        <v>86000</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.2">
@@ -3519,7 +3528,7 @@
         <v>86</v>
       </c>
       <c r="B108">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C108" t="s">
         <v>33</v>
@@ -3537,7 +3546,7 @@
         <v>14</v>
       </c>
       <c r="H108">
-        <v>118335</v>
+        <v>123000</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.2">
@@ -3545,7 +3554,7 @@
         <v>87</v>
       </c>
       <c r="B109">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C109" t="s">
         <v>35</v>
@@ -3563,7 +3572,7 @@
         <v>11</v>
       </c>
       <c r="H109">
-        <v>165000</v>
+        <v>168300</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.2">
@@ -3571,7 +3580,7 @@
         <v>88</v>
       </c>
       <c r="B110">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C110" t="s">
         <v>37</v>
@@ -3589,7 +3598,7 @@
         <v>11</v>
       </c>
       <c r="H110">
-        <v>163500</v>
+        <v>168800</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.2">
@@ -3597,7 +3606,7 @@
         <v>89</v>
       </c>
       <c r="B111">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C111" t="s">
         <v>39</v>
@@ -3615,7 +3624,7 @@
         <v>11</v>
       </c>
       <c r="H111">
-        <v>110000</v>
+        <v>112200</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.2">
@@ -3623,7 +3632,7 @@
         <v>90</v>
       </c>
       <c r="B112">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C112" t="s">
         <v>41</v>
@@ -3641,7 +3650,7 @@
         <v>14</v>
       </c>
       <c r="H112">
-        <v>84000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.2">
@@ -3649,7 +3658,7 @@
         <v>91</v>
       </c>
       <c r="B113">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C113" t="s">
         <v>43</v>
@@ -3667,7 +3676,7 @@
         <v>11</v>
       </c>
       <c r="H113">
-        <v>126500</v>
+        <v>143367</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.2">
@@ -3675,7 +3684,7 @@
         <v>92</v>
       </c>
       <c r="B114">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C114" t="s">
         <v>45</v>
@@ -3692,8 +3701,8 @@
       <c r="G114" t="s">
         <v>11</v>
       </c>
-      <c r="H114" t="s">
-        <v>73</v>
+      <c r="H114">
+        <v>152490</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.2">
@@ -3701,7 +3710,7 @@
         <v>93</v>
       </c>
       <c r="B115">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C115" t="s">
         <v>46</v>
@@ -3709,7 +3718,7 @@
       <c r="D115" t="s">
         <v>47</v>
       </c>
-      <c r="E115" s="1" t="s">
+      <c r="E115" t="s">
         <v>74</v>
       </c>
       <c r="F115">
@@ -3719,7 +3728,7 @@
         <v>14</v>
       </c>
       <c r="H115">
-        <v>101000</v>
+        <v>105000</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.2">
@@ -3727,7 +3736,7 @@
         <v>94</v>
       </c>
       <c r="B116">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C116" t="s">
         <v>48</v>
@@ -3745,7 +3754,7 @@
         <v>11</v>
       </c>
       <c r="H116">
-        <v>142300</v>
+        <v>145146</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.2">
@@ -3753,7 +3762,7 @@
         <v>95</v>
       </c>
       <c r="B117">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C117" t="s">
         <v>50</v>
@@ -3762,7 +3771,7 @@
         <v>51</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F117">
         <v>2015</v>
@@ -3771,7 +3780,7 @@
         <v>14</v>
       </c>
       <c r="H117">
-        <v>85000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.2">
@@ -3779,7 +3788,7 @@
         <v>96</v>
       </c>
       <c r="B118">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C118" t="s">
         <v>52</v>
@@ -3797,7 +3806,7 @@
         <v>14</v>
       </c>
       <c r="H118">
-        <v>226000</v>
+        <v>230000</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.2">
@@ -3805,7 +3814,7 @@
         <v>97</v>
       </c>
       <c r="B119">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C119" t="s">
         <v>54</v>
@@ -3823,7 +3832,7 @@
         <v>11</v>
       </c>
       <c r="H119">
-        <v>102960</v>
+        <v>105019</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.2">
@@ -3831,7 +3840,7 @@
         <v>98</v>
       </c>
       <c r="B120">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C120" t="s">
         <v>56</v>
@@ -3849,7 +3858,7 @@
         <v>11</v>
       </c>
       <c r="H120">
-        <v>100000</v>
+        <v>104000</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.2">
@@ -3857,7 +3866,7 @@
         <v>99</v>
       </c>
       <c r="B121">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C121" t="s">
         <v>58</v>
@@ -3875,7 +3884,7 @@
         <v>11</v>
       </c>
       <c r="H121">
-        <v>190000</v>
+        <v>195000</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.2">
@@ -3883,7 +3892,7 @@
         <v>100</v>
       </c>
       <c r="B122">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C122" t="s">
         <v>60</v>
@@ -3901,7 +3910,7 @@
         <v>11</v>
       </c>
       <c r="H122">
-        <v>84200</v>
+        <v>87000</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.2">
@@ -3909,7 +3918,7 @@
         <v>101</v>
       </c>
       <c r="B123">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C123" t="s">
         <v>62</v>
@@ -3927,7 +3936,7 @@
         <v>14</v>
       </c>
       <c r="H123">
-        <v>103000</v>
+        <v>105060</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.2">
@@ -3935,7 +3944,7 @@
         <v>102</v>
       </c>
       <c r="B124">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C124" t="s">
         <v>64</v>
@@ -3953,7 +3962,7 @@
         <v>14</v>
       </c>
       <c r="H124">
-        <v>100148</v>
+        <v>103148</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.2">
@@ -3961,7 +3970,7 @@
         <v>103</v>
       </c>
       <c r="B125">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C125" t="s">
         <v>48</v>
@@ -3979,7 +3988,7 @@
         <v>11</v>
       </c>
       <c r="H125">
-        <v>173538</v>
+        <v>178038</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.2">
@@ -3987,7 +3996,7 @@
         <v>104</v>
       </c>
       <c r="B126">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C126" t="s">
         <v>67</v>
@@ -4005,7 +4014,7 @@
         <v>11</v>
       </c>
       <c r="H126">
-        <v>106132</v>
+        <v>109316</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.2">
@@ -4013,7 +4022,7 @@
         <v>105</v>
       </c>
       <c r="B127">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C127" t="s">
         <v>69</v>
@@ -4031,7 +4040,7 @@
         <v>11</v>
       </c>
       <c r="H127">
-        <v>84200</v>
+        <v>87000</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.2">
@@ -4039,7 +4048,7 @@
         <v>106</v>
       </c>
       <c r="B128">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="C128" t="s">
         <v>71</v>
@@ -4057,7 +4066,7 @@
         <v>11</v>
       </c>
       <c r="H128">
-        <v>100917</v>
+        <v>104017</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.2">
@@ -4065,7 +4074,7 @@
         <v>75</v>
       </c>
       <c r="B129">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C129" t="s">
         <v>8</v>
@@ -4091,7 +4100,7 @@
         <v>76</v>
       </c>
       <c r="B130">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C130" t="s">
         <v>12</v>
@@ -4117,7 +4126,7 @@
         <v>77</v>
       </c>
       <c r="B131">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C131" t="s">
         <v>15</v>
@@ -4143,7 +4152,7 @@
         <v>78</v>
       </c>
       <c r="B132">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C132" t="s">
         <v>17</v>
@@ -4169,7 +4178,7 @@
         <v>79</v>
       </c>
       <c r="B133">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C133" t="s">
         <v>19</v>
@@ -4195,7 +4204,7 @@
         <v>80</v>
       </c>
       <c r="B134">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C134" t="s">
         <v>22</v>
@@ -4221,7 +4230,7 @@
         <v>81</v>
       </c>
       <c r="B135">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C135" t="s">
         <v>23</v>
@@ -4239,7 +4248,7 @@
         <v>14</v>
       </c>
       <c r="H135">
-        <v>90000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.2">
@@ -4247,7 +4256,7 @@
         <v>82</v>
       </c>
       <c r="B136">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C136" t="s">
         <v>25</v>
@@ -4265,7 +4274,7 @@
         <v>11</v>
       </c>
       <c r="H136">
-        <v>82000</v>
+        <v>84000</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.2">
@@ -4273,7 +4282,7 @@
         <v>83</v>
       </c>
       <c r="B137">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C137" t="s">
         <v>27</v>
@@ -4291,7 +4300,7 @@
         <v>14</v>
       </c>
       <c r="H137">
-        <v>97250</v>
+        <v>101250</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.2">
@@ -4299,7 +4308,7 @@
         <v>84</v>
       </c>
       <c r="B138">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C138" t="s">
         <v>29</v>
@@ -4317,7 +4326,7 @@
         <v>11</v>
       </c>
       <c r="H138">
-        <v>143000</v>
+        <v>144500</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.2">
@@ -4325,7 +4334,7 @@
         <v>85</v>
       </c>
       <c r="B139">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C139" t="s">
         <v>31</v>
@@ -4351,7 +4360,7 @@
         <v>86</v>
       </c>
       <c r="B140">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C140" t="s">
         <v>33</v>
@@ -4359,7 +4368,7 @@
       <c r="D140" t="s">
         <v>34</v>
       </c>
-      <c r="E140" t="s">
+      <c r="E140" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F140">
@@ -4369,7 +4378,7 @@
         <v>14</v>
       </c>
       <c r="H140">
-        <v>113335</v>
+        <v>118335</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.2">
@@ -4377,7 +4386,7 @@
         <v>87</v>
       </c>
       <c r="B141">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C141" t="s">
         <v>35</v>
@@ -4385,7 +4394,7 @@
       <c r="D141" t="s">
         <v>36</v>
       </c>
-      <c r="E141" t="s">
+      <c r="E141" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F141">
@@ -4395,7 +4404,7 @@
         <v>11</v>
       </c>
       <c r="H141">
-        <v>163000</v>
+        <v>165000</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.2">
@@ -4403,7 +4412,7 @@
         <v>88</v>
       </c>
       <c r="B142">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C142" t="s">
         <v>37</v>
@@ -4411,7 +4420,7 @@
       <c r="D142" t="s">
         <v>38</v>
       </c>
-      <c r="E142" t="s">
+      <c r="E142" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F142">
@@ -4421,7 +4430,7 @@
         <v>11</v>
       </c>
       <c r="H142">
-        <v>162000</v>
+        <v>163500</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.2">
@@ -4429,7 +4438,7 @@
         <v>89</v>
       </c>
       <c r="B143">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C143" t="s">
         <v>39</v>
@@ -4437,7 +4446,7 @@
       <c r="D143" t="s">
         <v>40</v>
       </c>
-      <c r="E143" t="s">
+      <c r="E143" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F143">
@@ -4446,8 +4455,8 @@
       <c r="G143" t="s">
         <v>11</v>
       </c>
-      <c r="H143" t="s">
-        <v>73</v>
+      <c r="H143">
+        <v>110000</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.2">
@@ -4455,7 +4464,7 @@
         <v>90</v>
       </c>
       <c r="B144">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C144" t="s">
         <v>41</v>
@@ -4463,7 +4472,7 @@
       <c r="D144" t="s">
         <v>42</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F144">
@@ -4473,7 +4482,7 @@
         <v>14</v>
       </c>
       <c r="H144">
-        <v>82000</v>
+        <v>84000</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.2">
@@ -4481,7 +4490,7 @@
         <v>91</v>
       </c>
       <c r="B145">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C145" t="s">
         <v>43</v>
@@ -4489,7 +4498,7 @@
       <c r="D145" t="s">
         <v>44</v>
       </c>
-      <c r="E145" t="s">
+      <c r="E145" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F145">
@@ -4499,7 +4508,7 @@
         <v>11</v>
       </c>
       <c r="H145">
-        <v>124444</v>
+        <v>126500</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.2">
@@ -4507,7 +4516,7 @@
         <v>92</v>
       </c>
       <c r="B146">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C146" t="s">
         <v>45</v>
@@ -4533,7 +4542,7 @@
         <v>93</v>
       </c>
       <c r="B147">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C147" t="s">
         <v>46</v>
@@ -4541,7 +4550,7 @@
       <c r="D147" t="s">
         <v>47</v>
       </c>
-      <c r="E147" t="s">
+      <c r="E147" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F147">
@@ -4551,7 +4560,7 @@
         <v>14</v>
       </c>
       <c r="H147">
-        <v>96500</v>
+        <v>101000</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.2">
@@ -4559,7 +4568,7 @@
         <v>94</v>
       </c>
       <c r="B148">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C148" t="s">
         <v>48</v>
@@ -4567,7 +4576,7 @@
       <c r="D148" t="s">
         <v>49</v>
       </c>
-      <c r="E148" t="s">
+      <c r="E148" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F148">
@@ -4577,7 +4586,7 @@
         <v>11</v>
       </c>
       <c r="H148">
-        <v>138100</v>
+        <v>142300</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.2">
@@ -4585,7 +4594,7 @@
         <v>95</v>
       </c>
       <c r="B149">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C149" t="s">
         <v>50</v>
@@ -4593,7 +4602,7 @@
       <c r="D149" t="s">
         <v>51</v>
       </c>
-      <c r="E149" t="s">
+      <c r="E149" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F149">
@@ -4603,7 +4612,7 @@
         <v>14</v>
       </c>
       <c r="H149">
-        <v>83000</v>
+        <v>85000</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.2">
@@ -4611,7 +4620,7 @@
         <v>96</v>
       </c>
       <c r="B150">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C150" t="s">
         <v>52</v>
@@ -4619,7 +4628,7 @@
       <c r="D150" t="s">
         <v>53</v>
       </c>
-      <c r="E150" t="s">
+      <c r="E150" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F150">
@@ -4629,7 +4638,7 @@
         <v>14</v>
       </c>
       <c r="H150">
-        <v>196000</v>
+        <v>226000</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.2">
@@ -4637,7 +4646,7 @@
         <v>97</v>
       </c>
       <c r="B151">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C151" t="s">
         <v>54</v>
@@ -4645,7 +4654,7 @@
       <c r="D151" t="s">
         <v>55</v>
       </c>
-      <c r="E151" t="s">
+      <c r="E151" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F151">
@@ -4655,7 +4664,7 @@
         <v>11</v>
       </c>
       <c r="H151">
-        <v>101460</v>
+        <v>102960</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.2">
@@ -4663,7 +4672,7 @@
         <v>98</v>
       </c>
       <c r="B152">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C152" t="s">
         <v>56</v>
@@ -4671,7 +4680,7 @@
       <c r="D152" t="s">
         <v>57</v>
       </c>
-      <c r="E152" t="s">
+      <c r="E152" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F152">
@@ -4681,7 +4690,7 @@
         <v>11</v>
       </c>
       <c r="H152">
-        <v>87000</v>
+        <v>100000</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.2">
@@ -4689,7 +4698,7 @@
         <v>99</v>
       </c>
       <c r="B153">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C153" t="s">
         <v>58</v>
@@ -4697,7 +4706,7 @@
       <c r="D153" t="s">
         <v>59</v>
       </c>
-      <c r="E153" t="s">
+      <c r="E153" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F153">
@@ -4707,7 +4716,7 @@
         <v>11</v>
       </c>
       <c r="H153">
-        <v>132000</v>
+        <v>190000</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.2">
@@ -4715,7 +4724,7 @@
         <v>100</v>
       </c>
       <c r="B154">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C154" t="s">
         <v>60</v>
@@ -4723,7 +4732,7 @@
       <c r="D154" t="s">
         <v>61</v>
       </c>
-      <c r="E154" t="s">
+      <c r="E154" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F154">
@@ -4733,7 +4742,7 @@
         <v>11</v>
       </c>
       <c r="H154">
-        <v>82200</v>
+        <v>84200</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.2">
@@ -4741,7 +4750,7 @@
         <v>101</v>
       </c>
       <c r="B155">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C155" t="s">
         <v>62</v>
@@ -4749,7 +4758,7 @@
       <c r="D155" t="s">
         <v>63</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F155">
@@ -4759,7 +4768,7 @@
         <v>14</v>
       </c>
       <c r="H155">
-        <v>99000</v>
+        <v>103000</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.2">
@@ -4767,7 +4776,7 @@
         <v>102</v>
       </c>
       <c r="B156">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C156" t="s">
         <v>64</v>
@@ -4775,7 +4784,7 @@
       <c r="D156" t="s">
         <v>65</v>
       </c>
-      <c r="E156" t="s">
+      <c r="E156" s="1" t="s">
         <v>74</v>
       </c>
       <c r="F156">
@@ -4785,7 +4794,7 @@
         <v>14</v>
       </c>
       <c r="H156">
-        <v>95148</v>
+        <v>100148</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.2">
@@ -4793,7 +4802,7 @@
         <v>103</v>
       </c>
       <c r="B157">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C157" t="s">
         <v>48</v>
@@ -4801,7 +4810,7 @@
       <c r="D157" t="s">
         <v>66</v>
       </c>
-      <c r="E157" t="s">
+      <c r="E157" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F157">
@@ -4811,7 +4820,7 @@
         <v>11</v>
       </c>
       <c r="H157">
-        <v>154256</v>
+        <v>173538</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.2">
@@ -4819,7 +4828,7 @@
         <v>104</v>
       </c>
       <c r="B158">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C158" t="s">
         <v>67</v>
@@ -4837,7 +4846,7 @@
         <v>11</v>
       </c>
       <c r="H158">
-        <v>104132</v>
+        <v>106132</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.2">
@@ -4845,7 +4854,7 @@
         <v>105</v>
       </c>
       <c r="B159">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C159" t="s">
         <v>69</v>
@@ -4863,7 +4872,7 @@
         <v>11</v>
       </c>
       <c r="H159">
-        <v>82200</v>
+        <v>84200</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.2">
@@ -4871,7 +4880,7 @@
         <v>106</v>
       </c>
       <c r="B160">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="C160" t="s">
         <v>71</v>
@@ -4889,7 +4898,7 @@
         <v>11</v>
       </c>
       <c r="H160">
-        <v>95917</v>
+        <v>100917</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.2">
@@ -4897,7 +4906,7 @@
         <v>75</v>
       </c>
       <c r="B161">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C161" t="s">
         <v>8</v>
@@ -4923,7 +4932,7 @@
         <v>76</v>
       </c>
       <c r="B162">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C162" t="s">
         <v>12</v>
@@ -4949,7 +4958,7 @@
         <v>77</v>
       </c>
       <c r="B163">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C163" t="s">
         <v>15</v>
@@ -4975,7 +4984,7 @@
         <v>78</v>
       </c>
       <c r="B164">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C164" t="s">
         <v>17</v>
@@ -5001,7 +5010,7 @@
         <v>79</v>
       </c>
       <c r="B165">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C165" t="s">
         <v>19</v>
@@ -5027,7 +5036,7 @@
         <v>80</v>
       </c>
       <c r="B166">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C166" t="s">
         <v>22</v>
@@ -5053,7 +5062,7 @@
         <v>81</v>
       </c>
       <c r="B167">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C167" t="s">
         <v>23</v>
@@ -5062,7 +5071,7 @@
         <v>24</v>
       </c>
       <c r="E167" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F167">
         <v>2012</v>
@@ -5071,7 +5080,7 @@
         <v>14</v>
       </c>
       <c r="H167">
-        <v>76000</v>
+        <v>90000</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.2">
@@ -5079,7 +5088,7 @@
         <v>82</v>
       </c>
       <c r="B168">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C168" t="s">
         <v>25</v>
@@ -5096,8 +5105,8 @@
       <c r="G168" t="s">
         <v>11</v>
       </c>
-      <c r="H168" t="s">
-        <v>73</v>
+      <c r="H168">
+        <v>82000</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.2">
@@ -5105,7 +5114,7 @@
         <v>83</v>
       </c>
       <c r="B169">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C169" t="s">
         <v>27</v>
@@ -5123,7 +5132,7 @@
         <v>14</v>
       </c>
       <c r="H169">
-        <v>90250</v>
+        <v>97250</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.2">
@@ -5131,7 +5140,7 @@
         <v>84</v>
       </c>
       <c r="B170">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C170" t="s">
         <v>29</v>
@@ -5139,7 +5148,7 @@
       <c r="D170" t="s">
         <v>30</v>
       </c>
-      <c r="E170" t="s">
+      <c r="E170" s="1" t="s">
         <v>21</v>
       </c>
       <c r="F170">
@@ -5149,7 +5158,7 @@
         <v>11</v>
       </c>
       <c r="H170">
-        <v>137500</v>
+        <v>143000</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -5157,7 +5166,7 @@
         <v>85</v>
       </c>
       <c r="B171">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C171" t="s">
         <v>31</v>
@@ -5183,7 +5192,7 @@
         <v>86</v>
       </c>
       <c r="B172">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C172" t="s">
         <v>33</v>
@@ -5201,7 +5210,7 @@
         <v>14</v>
       </c>
       <c r="H172">
-        <v>106335</v>
+        <v>113335</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -5209,7 +5218,7 @@
         <v>87</v>
       </c>
       <c r="B173">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C173" t="s">
         <v>35</v>
@@ -5227,7 +5236,7 @@
         <v>11</v>
       </c>
       <c r="H173">
-        <v>161000</v>
+        <v>163000</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -5235,7 +5244,7 @@
         <v>88</v>
       </c>
       <c r="B174">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C174" t="s">
         <v>37</v>
@@ -5253,7 +5262,7 @@
         <v>11</v>
       </c>
       <c r="H174">
-        <v>160000</v>
+        <v>162000</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -5261,7 +5270,7 @@
         <v>89</v>
       </c>
       <c r="B175">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C175" t="s">
         <v>39</v>
@@ -5287,7 +5296,7 @@
         <v>90</v>
       </c>
       <c r="B176">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C176" t="s">
         <v>41</v>
@@ -5304,8 +5313,8 @@
       <c r="G176" t="s">
         <v>14</v>
       </c>
-      <c r="H176" t="s">
-        <v>73</v>
+      <c r="H176">
+        <v>82000</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -5313,7 +5322,7 @@
         <v>91</v>
       </c>
       <c r="B177">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C177" t="s">
         <v>43</v>
@@ -5322,7 +5331,7 @@
         <v>44</v>
       </c>
       <c r="E177" t="s">
-        <v>74</v>
+        <v>21</v>
       </c>
       <c r="F177">
         <v>2015</v>
@@ -5331,7 +5340,7 @@
         <v>11</v>
       </c>
       <c r="H177">
-        <v>122222</v>
+        <v>124444</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -5339,7 +5348,7 @@
         <v>92</v>
       </c>
       <c r="B178">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C178" t="s">
         <v>45</v>
@@ -5365,7 +5374,7 @@
         <v>93</v>
       </c>
       <c r="B179">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C179" t="s">
         <v>46</v>
@@ -5383,7 +5392,7 @@
         <v>14</v>
       </c>
       <c r="H179">
-        <v>92500</v>
+        <v>96500</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -5391,7 +5400,7 @@
         <v>94</v>
       </c>
       <c r="B180">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C180" t="s">
         <v>48</v>
@@ -5409,7 +5418,7 @@
         <v>11</v>
       </c>
       <c r="H180">
-        <v>129100</v>
+        <v>138100</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -5417,7 +5426,7 @@
         <v>95</v>
       </c>
       <c r="B181">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C181" t="s">
         <v>50</v>
@@ -5435,7 +5444,7 @@
         <v>14</v>
       </c>
       <c r="H181">
-        <v>76000</v>
+        <v>83000</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -5443,7 +5452,7 @@
         <v>96</v>
       </c>
       <c r="B182">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C182" t="s">
         <v>52</v>
@@ -5461,7 +5470,7 @@
         <v>14</v>
       </c>
       <c r="H182">
-        <v>190000</v>
+        <v>196000</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -5469,7 +5478,7 @@
         <v>97</v>
       </c>
       <c r="B183">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C183" t="s">
         <v>54</v>
@@ -5495,7 +5504,7 @@
         <v>98</v>
       </c>
       <c r="B184">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C184" t="s">
         <v>56</v>
@@ -5504,7 +5513,7 @@
         <v>57</v>
       </c>
       <c r="E184" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="F184">
         <v>2013</v>
@@ -5513,7 +5522,7 @@
         <v>11</v>
       </c>
       <c r="H184">
-        <v>83000</v>
+        <v>87000</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -5521,7 +5530,7 @@
         <v>99</v>
       </c>
       <c r="B185">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C185" t="s">
         <v>58</v>
@@ -5539,7 +5548,7 @@
         <v>11</v>
       </c>
       <c r="H185">
-        <v>129000</v>
+        <v>132000</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -5547,7 +5556,7 @@
         <v>100</v>
       </c>
       <c r="B186">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C186" t="s">
         <v>60</v>
@@ -5565,7 +5574,7 @@
         <v>11</v>
       </c>
       <c r="H186">
-        <v>76000</v>
+        <v>82200</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -5573,7 +5582,7 @@
         <v>101</v>
       </c>
       <c r="B187">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C187" t="s">
         <v>62</v>
@@ -5591,7 +5600,7 @@
         <v>14</v>
       </c>
       <c r="H187">
-        <v>88300</v>
+        <v>99000</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -5599,7 +5608,7 @@
         <v>102</v>
       </c>
       <c r="B188">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C188" t="s">
         <v>64</v>
@@ -5617,7 +5626,7 @@
         <v>14</v>
       </c>
       <c r="H188">
-        <v>88148</v>
+        <v>95148</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -5625,7 +5634,7 @@
         <v>103</v>
       </c>
       <c r="B189">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C189" t="s">
         <v>48</v>
@@ -5643,7 +5652,7 @@
         <v>11</v>
       </c>
       <c r="H189">
-        <v>147256</v>
+        <v>154256</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -5651,7 +5660,7 @@
         <v>104</v>
       </c>
       <c r="B190">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C190" t="s">
         <v>67</v>
@@ -5669,7 +5678,7 @@
         <v>11</v>
       </c>
       <c r="H190">
-        <v>101632</v>
+        <v>104132</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
@@ -5677,7 +5686,7 @@
         <v>105</v>
       </c>
       <c r="B191">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C191" t="s">
         <v>69</v>
@@ -5695,7 +5704,7 @@
         <v>11</v>
       </c>
       <c r="H191">
-        <v>76000</v>
+        <v>82200</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
@@ -5703,7 +5712,7 @@
         <v>106</v>
       </c>
       <c r="B192">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="C192" t="s">
         <v>71</v>
@@ -5721,6 +5730,838 @@
         <v>11</v>
       </c>
       <c r="H192">
+        <v>95917</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>75</v>
+      </c>
+      <c r="B193">
+        <v>2018</v>
+      </c>
+      <c r="C193" t="s">
+        <v>8</v>
+      </c>
+      <c r="D193" t="s">
+        <v>9</v>
+      </c>
+      <c r="E193" t="s">
+        <v>10</v>
+      </c>
+      <c r="F193">
+        <v>2022</v>
+      </c>
+      <c r="G193" t="s">
+        <v>11</v>
+      </c>
+      <c r="H193" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>76</v>
+      </c>
+      <c r="B194">
+        <v>2018</v>
+      </c>
+      <c r="C194" t="s">
+        <v>12</v>
+      </c>
+      <c r="D194" t="s">
+        <v>13</v>
+      </c>
+      <c r="E194" t="s">
+        <v>10</v>
+      </c>
+      <c r="F194">
+        <v>2022</v>
+      </c>
+      <c r="G194" t="s">
+        <v>14</v>
+      </c>
+      <c r="H194" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>77</v>
+      </c>
+      <c r="B195">
+        <v>2018</v>
+      </c>
+      <c r="C195" t="s">
+        <v>15</v>
+      </c>
+      <c r="D195" t="s">
+        <v>16</v>
+      </c>
+      <c r="E195" t="s">
+        <v>10</v>
+      </c>
+      <c r="F195">
+        <v>2022</v>
+      </c>
+      <c r="G195" t="s">
+        <v>14</v>
+      </c>
+      <c r="H195" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>78</v>
+      </c>
+      <c r="B196">
+        <v>2018</v>
+      </c>
+      <c r="C196" t="s">
+        <v>17</v>
+      </c>
+      <c r="D196" t="s">
+        <v>18</v>
+      </c>
+      <c r="E196" t="s">
+        <v>10</v>
+      </c>
+      <c r="F196">
+        <v>2022</v>
+      </c>
+      <c r="G196" t="s">
+        <v>11</v>
+      </c>
+      <c r="H196" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>79</v>
+      </c>
+      <c r="B197">
+        <v>2018</v>
+      </c>
+      <c r="C197" t="s">
+        <v>19</v>
+      </c>
+      <c r="D197" t="s">
+        <v>20</v>
+      </c>
+      <c r="E197" t="s">
+        <v>21</v>
+      </c>
+      <c r="F197">
+        <v>2022</v>
+      </c>
+      <c r="G197" t="s">
+        <v>11</v>
+      </c>
+      <c r="H197" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>80</v>
+      </c>
+      <c r="B198">
+        <v>2018</v>
+      </c>
+      <c r="C198" t="s">
+        <v>22</v>
+      </c>
+      <c r="D198" t="s">
+        <v>107</v>
+      </c>
+      <c r="E198" t="s">
+        <v>21</v>
+      </c>
+      <c r="F198">
+        <v>2022</v>
+      </c>
+      <c r="G198" t="s">
+        <v>14</v>
+      </c>
+      <c r="H198" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>81</v>
+      </c>
+      <c r="B199">
+        <v>2018</v>
+      </c>
+      <c r="C199" t="s">
+        <v>23</v>
+      </c>
+      <c r="D199" t="s">
+        <v>24</v>
+      </c>
+      <c r="E199" t="s">
+        <v>10</v>
+      </c>
+      <c r="F199">
+        <v>2012</v>
+      </c>
+      <c r="G199" t="s">
+        <v>14</v>
+      </c>
+      <c r="H199">
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>82</v>
+      </c>
+      <c r="B200">
+        <v>2018</v>
+      </c>
+      <c r="C200" t="s">
+        <v>25</v>
+      </c>
+      <c r="D200" t="s">
+        <v>26</v>
+      </c>
+      <c r="E200" t="s">
+        <v>10</v>
+      </c>
+      <c r="F200">
+        <v>2018</v>
+      </c>
+      <c r="G200" t="s">
+        <v>11</v>
+      </c>
+      <c r="H200" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>83</v>
+      </c>
+      <c r="B201">
+        <v>2018</v>
+      </c>
+      <c r="C201" t="s">
+        <v>27</v>
+      </c>
+      <c r="D201" t="s">
+        <v>28</v>
+      </c>
+      <c r="E201" t="s">
+        <v>74</v>
+      </c>
+      <c r="F201">
+        <v>2012</v>
+      </c>
+      <c r="G201" t="s">
+        <v>14</v>
+      </c>
+      <c r="H201">
+        <v>90250</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>84</v>
+      </c>
+      <c r="B202">
+        <v>2018</v>
+      </c>
+      <c r="C202" t="s">
+        <v>29</v>
+      </c>
+      <c r="D202" t="s">
+        <v>30</v>
+      </c>
+      <c r="E202" t="s">
+        <v>21</v>
+      </c>
+      <c r="F202">
+        <v>2014</v>
+      </c>
+      <c r="G202" t="s">
+        <v>11</v>
+      </c>
+      <c r="H202">
+        <v>137500</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>85</v>
+      </c>
+      <c r="B203">
+        <v>2018</v>
+      </c>
+      <c r="C203" t="s">
+        <v>31</v>
+      </c>
+      <c r="D203" t="s">
+        <v>32</v>
+      </c>
+      <c r="E203" t="s">
+        <v>10</v>
+      </c>
+      <c r="F203">
+        <v>2020</v>
+      </c>
+      <c r="G203" t="s">
+        <v>14</v>
+      </c>
+      <c r="H203" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>86</v>
+      </c>
+      <c r="B204">
+        <v>2018</v>
+      </c>
+      <c r="C204" t="s">
+        <v>33</v>
+      </c>
+      <c r="D204" t="s">
+        <v>34</v>
+      </c>
+      <c r="E204" t="s">
+        <v>21</v>
+      </c>
+      <c r="F204">
+        <v>2008</v>
+      </c>
+      <c r="G204" t="s">
+        <v>14</v>
+      </c>
+      <c r="H204">
+        <v>106335</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>87</v>
+      </c>
+      <c r="B205">
+        <v>2018</v>
+      </c>
+      <c r="C205" t="s">
+        <v>35</v>
+      </c>
+      <c r="D205" t="s">
+        <v>36</v>
+      </c>
+      <c r="E205" t="s">
+        <v>21</v>
+      </c>
+      <c r="F205">
+        <v>1997</v>
+      </c>
+      <c r="G205" t="s">
+        <v>11</v>
+      </c>
+      <c r="H205">
+        <v>161000</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>88</v>
+      </c>
+      <c r="B206">
+        <v>2018</v>
+      </c>
+      <c r="C206" t="s">
+        <v>37</v>
+      </c>
+      <c r="D206" t="s">
+        <v>38</v>
+      </c>
+      <c r="E206" t="s">
+        <v>21</v>
+      </c>
+      <c r="F206">
+        <v>2016</v>
+      </c>
+      <c r="G206" t="s">
+        <v>11</v>
+      </c>
+      <c r="H206">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>89</v>
+      </c>
+      <c r="B207">
+        <v>2018</v>
+      </c>
+      <c r="C207" t="s">
+        <v>39</v>
+      </c>
+      <c r="D207" t="s">
+        <v>40</v>
+      </c>
+      <c r="E207" t="s">
+        <v>74</v>
+      </c>
+      <c r="F207">
+        <v>2020</v>
+      </c>
+      <c r="G207" t="s">
+        <v>11</v>
+      </c>
+      <c r="H207" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>90</v>
+      </c>
+      <c r="B208">
+        <v>2018</v>
+      </c>
+      <c r="C208" t="s">
+        <v>41</v>
+      </c>
+      <c r="D208" t="s">
+        <v>42</v>
+      </c>
+      <c r="E208" t="s">
+        <v>10</v>
+      </c>
+      <c r="F208">
+        <v>2018</v>
+      </c>
+      <c r="G208" t="s">
+        <v>14</v>
+      </c>
+      <c r="H208" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>91</v>
+      </c>
+      <c r="B209">
+        <v>2018</v>
+      </c>
+      <c r="C209" t="s">
+        <v>43</v>
+      </c>
+      <c r="D209" t="s">
+        <v>44</v>
+      </c>
+      <c r="E209" t="s">
+        <v>74</v>
+      </c>
+      <c r="F209">
+        <v>2015</v>
+      </c>
+      <c r="G209" t="s">
+        <v>11</v>
+      </c>
+      <c r="H209">
+        <v>122222</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>92</v>
+      </c>
+      <c r="B210">
+        <v>2018</v>
+      </c>
+      <c r="C210" t="s">
+        <v>45</v>
+      </c>
+      <c r="D210" t="s">
+        <v>108</v>
+      </c>
+      <c r="E210" t="s">
+        <v>21</v>
+      </c>
+      <c r="F210">
+        <v>2020</v>
+      </c>
+      <c r="G210" t="s">
+        <v>11</v>
+      </c>
+      <c r="H210" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>93</v>
+      </c>
+      <c r="B211">
+        <v>2018</v>
+      </c>
+      <c r="C211" t="s">
+        <v>46</v>
+      </c>
+      <c r="D211" t="s">
+        <v>47</v>
+      </c>
+      <c r="E211" t="s">
+        <v>74</v>
+      </c>
+      <c r="F211">
+        <v>2015</v>
+      </c>
+      <c r="G211" t="s">
+        <v>14</v>
+      </c>
+      <c r="H211">
+        <v>92500</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>94</v>
+      </c>
+      <c r="B212">
+        <v>2018</v>
+      </c>
+      <c r="C212" t="s">
+        <v>48</v>
+      </c>
+      <c r="D212" t="s">
+        <v>49</v>
+      </c>
+      <c r="E212" t="s">
+        <v>21</v>
+      </c>
+      <c r="F212">
+        <v>2008</v>
+      </c>
+      <c r="G212" t="s">
+        <v>11</v>
+      </c>
+      <c r="H212">
+        <v>129100</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>95</v>
+      </c>
+      <c r="B213">
+        <v>2018</v>
+      </c>
+      <c r="C213" t="s">
+        <v>50</v>
+      </c>
+      <c r="D213" t="s">
+        <v>51</v>
+      </c>
+      <c r="E213" t="s">
+        <v>10</v>
+      </c>
+      <c r="F213">
+        <v>2015</v>
+      </c>
+      <c r="G213" t="s">
+        <v>14</v>
+      </c>
+      <c r="H213">
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>96</v>
+      </c>
+      <c r="B214">
+        <v>2018</v>
+      </c>
+      <c r="C214" t="s">
+        <v>52</v>
+      </c>
+      <c r="D214" t="s">
+        <v>53</v>
+      </c>
+      <c r="E214" t="s">
+        <v>21</v>
+      </c>
+      <c r="F214">
+        <v>2006</v>
+      </c>
+      <c r="G214" t="s">
+        <v>14</v>
+      </c>
+      <c r="H214">
+        <v>190000</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>97</v>
+      </c>
+      <c r="B215">
+        <v>2018</v>
+      </c>
+      <c r="C215" t="s">
+        <v>54</v>
+      </c>
+      <c r="D215" t="s">
+        <v>55</v>
+      </c>
+      <c r="E215" t="s">
+        <v>74</v>
+      </c>
+      <c r="F215">
+        <v>2006</v>
+      </c>
+      <c r="G215" t="s">
+        <v>11</v>
+      </c>
+      <c r="H215">
+        <v>101460</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>98</v>
+      </c>
+      <c r="B216">
+        <v>2018</v>
+      </c>
+      <c r="C216" t="s">
+        <v>56</v>
+      </c>
+      <c r="D216" t="s">
+        <v>57</v>
+      </c>
+      <c r="E216" t="s">
+        <v>10</v>
+      </c>
+      <c r="F216">
+        <v>2013</v>
+      </c>
+      <c r="G216" t="s">
+        <v>11</v>
+      </c>
+      <c r="H216">
+        <v>83000</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>99</v>
+      </c>
+      <c r="B217">
+        <v>2018</v>
+      </c>
+      <c r="C217" t="s">
+        <v>58</v>
+      </c>
+      <c r="D217" t="s">
+        <v>59</v>
+      </c>
+      <c r="E217" t="s">
+        <v>21</v>
+      </c>
+      <c r="F217">
+        <v>2015</v>
+      </c>
+      <c r="G217" t="s">
+        <v>11</v>
+      </c>
+      <c r="H217">
+        <v>129000</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>100</v>
+      </c>
+      <c r="B218">
+        <v>2018</v>
+      </c>
+      <c r="C218" t="s">
+        <v>60</v>
+      </c>
+      <c r="D218" t="s">
+        <v>61</v>
+      </c>
+      <c r="E218" t="s">
+        <v>10</v>
+      </c>
+      <c r="F218">
+        <v>2016</v>
+      </c>
+      <c r="G218" t="s">
+        <v>11</v>
+      </c>
+      <c r="H218">
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>101</v>
+      </c>
+      <c r="B219">
+        <v>2018</v>
+      </c>
+      <c r="C219" t="s">
+        <v>62</v>
+      </c>
+      <c r="D219" t="s">
+        <v>63</v>
+      </c>
+      <c r="E219" t="s">
+        <v>74</v>
+      </c>
+      <c r="F219">
+        <v>2009</v>
+      </c>
+      <c r="G219" t="s">
+        <v>14</v>
+      </c>
+      <c r="H219">
+        <v>88300</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>102</v>
+      </c>
+      <c r="B220">
+        <v>2018</v>
+      </c>
+      <c r="C220" t="s">
+        <v>64</v>
+      </c>
+      <c r="D220" t="s">
+        <v>65</v>
+      </c>
+      <c r="E220" t="s">
+        <v>74</v>
+      </c>
+      <c r="F220">
+        <v>2008</v>
+      </c>
+      <c r="G220" t="s">
+        <v>14</v>
+      </c>
+      <c r="H220">
+        <v>88148</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>103</v>
+      </c>
+      <c r="B221">
+        <v>2018</v>
+      </c>
+      <c r="C221" t="s">
+        <v>48</v>
+      </c>
+      <c r="D221" t="s">
+        <v>66</v>
+      </c>
+      <c r="E221" t="s">
+        <v>21</v>
+      </c>
+      <c r="F221">
+        <v>2008</v>
+      </c>
+      <c r="G221" t="s">
+        <v>11</v>
+      </c>
+      <c r="H221">
+        <v>147256</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>104</v>
+      </c>
+      <c r="B222">
+        <v>2018</v>
+      </c>
+      <c r="C222" t="s">
+        <v>67</v>
+      </c>
+      <c r="D222" t="s">
+        <v>68</v>
+      </c>
+      <c r="E222" t="s">
+        <v>74</v>
+      </c>
+      <c r="F222">
+        <v>2010</v>
+      </c>
+      <c r="G222" t="s">
+        <v>11</v>
+      </c>
+      <c r="H222">
+        <v>101632</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>105</v>
+      </c>
+      <c r="B223">
+        <v>2018</v>
+      </c>
+      <c r="C223" t="s">
+        <v>69</v>
+      </c>
+      <c r="D223" t="s">
+        <v>70</v>
+      </c>
+      <c r="E223" t="s">
+        <v>10</v>
+      </c>
+      <c r="F223">
+        <v>2016</v>
+      </c>
+      <c r="G223" t="s">
+        <v>11</v>
+      </c>
+      <c r="H223">
+        <v>76000</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>106</v>
+      </c>
+      <c r="B224">
+        <v>2018</v>
+      </c>
+      <c r="C224" t="s">
+        <v>71</v>
+      </c>
+      <c r="D224" t="s">
+        <v>72</v>
+      </c>
+      <c r="E224" t="s">
+        <v>74</v>
+      </c>
+      <c r="F224">
+        <v>2011</v>
+      </c>
+      <c r="G224" t="s">
+        <v>11</v>
+      </c>
+      <c r="H224">
         <v>88917</v>
       </c>
     </row>

</xml_diff>